<commit_message>
adding units to concentrations
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_check_model_model.xlsx
+++ b/tests/fixtures/test_check_model_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,26 +37,31 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -68,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="137">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -265,9 +270,15 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
     <t xml:space="preserve">specie_1[e]</t>
   </si>
   <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
     <t xml:space="preserve">specie_2[e]</t>
   </si>
   <si>
@@ -410,9 +421,6 @@
   </si>
   <si>
     <t xml:space="preserve">Submodels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
   </si>
   <si>
     <t xml:space="preserve">fractionDryWeight</t>
@@ -743,14 +751,14 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C2:C7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -837,31 +845,31 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="1" sqref="C2:C7 C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.3117408906883"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.6032388663968"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -872,24 +880,26 @@
     </row>
     <row r="2" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>2000</v>
@@ -898,13 +908,13 @@
     </row>
     <row r="4" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>0.0003</v>
@@ -915,13 +925,13 @@
     </row>
     <row r="5" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>0.0003</v>
@@ -932,13 +942,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>0.0003</v>
@@ -966,14 +976,14 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="C2:C7 C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="10" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="20.995951417004"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="10" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="10" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="10" width="9.31983805668016"/>
@@ -992,10 +1002,10 @@
         <v>22</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>13</v>
@@ -1006,10 +1016,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>28</v>
@@ -1021,16 +1031,16 @@
         <v>44</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>28</v>
@@ -1044,10 +1054,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>28</v>
@@ -1078,13 +1088,13 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="1" sqref="C2:C7 C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="10" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="10" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="10" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -1110,13 +1120,13 @@
         <v>28</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1138,17 +1148,17 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="1" sqref="C2:C7 B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="43.5991902834008"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="43.919028340081"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="49.165991902834"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="49.4898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -1160,16 +1170,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>13</v>
@@ -1180,10 +1190,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -1192,10 +1202,10 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1219,7 +1229,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M39" activeCellId="0" sqref="M39"/>
+      <selection pane="topLeft" activeCell="M39" activeCellId="1" sqref="C2:C7 M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1235,7 +1245,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1260,15 +1270,15 @@
   <dimension ref="1:1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="1" sqref="C2:C7 F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="15.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="31.8137651821862"/>
     <col collapsed="false" hidden="false" max="1023" min="5" style="3" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="8.78542510121457"/>
   </cols>
@@ -1281,46 +1291,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>43</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>13</v>
@@ -1348,7 +1358,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="C2:C7 E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1358,34 +1368,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1407,7 +1417,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+      <selection pane="topLeft" activeCell="C36" activeCellId="1" sqref="C2:C7 C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1471,16 +1481,16 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="1" sqref="C2:C7 F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="3" width="13.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="3" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="3" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="3" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="1023" min="9" style="3" width="8.78542510121457"/>
@@ -1565,15 +1575,15 @@
   <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="1" sqref="C2:C7 D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="5.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="45.5263157894737"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.8178137651822"/>
     <col collapsed="false" hidden="false" max="1023" min="6" style="3" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="8.78542510121457"/>
@@ -1646,18 +1656,18 @@
   <dimension ref="1:7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="1" sqref="C2:C7 E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="3" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="3" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="3" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="3" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="1023" min="10" style="3" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="8.78542510121457"/>
@@ -1836,24 +1846,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="3" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="3" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="3" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="3" width="9.31983805668016"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="3" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="3" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="3" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1864,58 +1874,79 @@
         <v>64</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>0.000148</v>
       </c>
+      <c r="C2" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>0.0002</v>
       </c>
+      <c r="C3" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C4" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>0.0005</v>
       </c>
+      <c r="C5" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>0.001</v>
       </c>
+      <c r="C6" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>0.002</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1937,7 +1968,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G39" activeCellId="0" sqref="G39"/>
+      <selection pane="topLeft" activeCell="G39" activeCellId="1" sqref="C2:C7 G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1956,7 +1987,7 @@
         <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
@@ -1981,7 +2012,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+      <selection pane="topLeft" activeCell="H34" activeCellId="1" sqref="C2:C7 H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1997,7 +2028,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -2022,15 +2053,15 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="C2:C7 B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="3" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="45.8461538461538"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="1" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="3" width="11.7813765182186"/>
@@ -2046,19 +2077,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -2069,16 +2100,16 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>0</v>
@@ -2094,16 +2125,16 @@
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
@@ -2119,16 +2150,16 @@
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -2138,16 +2169,16 @@
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
changing Species formatting so that Species must be explicitly defined in XLSX files and Species have ids
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_check_model_model.xlsx
+++ b/tests/fixtures/test_check_model_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,23 +13,24 @@
     <sheet name="Submodels" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Compartments" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Species types" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Concentrations" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Observables" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="Functions" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="Reactions" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Rate laws" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Biomass components" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Biomass reactions" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Parameters" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Stop conditions" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="References" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="Database references" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Species" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Concentrations" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Observables" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Rate laws" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Biomass components" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Biomass reactions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Parameters" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Stop conditions" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="References" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="Database references" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="true" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
@@ -38,30 +39,55 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -73,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="138">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -261,6 +287,36 @@
     <t xml:space="preserve">U238</t>
   </si>
   <si>
+    <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_3[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_6[c]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Species</t>
   </si>
   <si>
@@ -270,27 +326,9 @@
     <t xml:space="preserve">Units</t>
   </si>
   <si>
-    <t xml:space="preserve">specie_1[e]</t>
-  </si>
-  <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">specie_2[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_6[c]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Expression</t>
   </si>
   <si>
@@ -381,9 +419,6 @@
     <t xml:space="preserve">Coefficient</t>
   </si>
   <si>
-    <t xml:space="preserve">Species type</t>
-  </si>
-  <si>
     <t xml:space="preserve">biomass_id_001</t>
   </si>
   <si>
@@ -403,9 +438,6 @@
   </si>
   <si>
     <t xml:space="preserve">biomass_comp_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compartment</t>
   </si>
   <si>
     <t xml:space="preserve">Metabolism biomass reaction</t>
@@ -493,7 +525,7 @@
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -528,6 +560,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -591,7 +631,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -622,6 +662,14 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -838,6 +886,155 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="5" min="1" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D5"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -852,19 +1049,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -875,26 +1072,26 @@
     </row>
     <row r="2" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>2000</v>
@@ -903,13 +1100,13 @@
     </row>
     <row r="4" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>0.0003</v>
@@ -920,13 +1117,13 @@
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>0.0003</v>
@@ -937,13 +1134,13 @@
     </row>
     <row r="6" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>0.0003</v>
@@ -963,7 +1160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -976,65 +1173,65 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="10" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="12" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="A2" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="13" t="n">
+      <c r="D2" s="15" t="n">
         <v>-3</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="12"/>
+      <c r="F2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="13" t="n">
+      <c r="D3" s="15" t="n">
         <v>-4</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1042,16 +1239,16 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="A4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="15" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1069,7 +1266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1082,24 +1279,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="10" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="12" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="C1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1107,14 +1304,14 @@
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>112</v>
+      <c r="D2" s="12" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1128,7 +1325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1153,16 +1350,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>13</v>
@@ -1173,10 +1370,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -1185,10 +1382,10 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1204,7 +1401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1229,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1246,7 +1443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1271,46 +1468,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>13</v>
@@ -1330,7 +1527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1349,34 +1546,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1462,7 +1659,7 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1804,13 +2001,153 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B13" activeCellId="0" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="5" min="1" style="3" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
@@ -1818,13 +2155,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -1835,35 +2172,35 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>0.000148</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>0.0002</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>0.0005</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1874,7 +2211,7 @@
         <v>0.0005</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1885,7 +2222,7 @@
         <v>0.001</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1896,7 +2233,7 @@
         <v>0.002</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1910,7 +2247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1935,7 +2272,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1952,7 +2289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1977,7 +2314,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1992,153 +2329,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="4" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D5"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
refactoring relationship between Submodel and BiomassReaction
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_check_model_model.xlsx
+++ b/tests/fixtures/test_check_model_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,8 +19,8 @@
     <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Rate laws" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Biomass components" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Biomass reactions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Biomass reactions" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Biomass components" sheetId="13" state="visible" r:id="rId14"/>
     <sheet name="Parameters" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Stop conditions" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="References" sheetId="16" state="visible" r:id="rId17"/>
@@ -44,6 +44,9 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
@@ -55,6 +58,9 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -66,6 +72,9 @@
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
@@ -77,6 +86,9 @@
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -88,6 +100,9 @@
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -99,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="138">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -164,258 +179,264 @@
     <t xml:space="preserve">Algorithm</t>
   </si>
   <si>
+    <t xml:space="preserve">Objective function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba_submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2*Metabolism_biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssa_submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracellular space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typical density of Mycoplasma pneumoniae cells in culture is 1e-9 cells/mL [Ref-0002].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empirical formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molecular weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pseudo_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N2O2Na3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3SO4C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_3[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_6[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max flux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; specie_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_name_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K cat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat * specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4[c] / k_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">backward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism_biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism biomass reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No comment</t>
+  </si>
+  <si>
     <t xml:space="preserve">Biomass reaction</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba_submodel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism_biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2*Metabolism_biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssa_submodel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extracellular space</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typical density of Mycoplasma pneumoniae cells in culture is 1e-9 cells/mL [Ref-0002].</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empirical formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molecular weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pseudo_species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2O2Na3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H3SO4C9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_3[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_6[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submodel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reversible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Min flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max flux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[e] + specie_2[e] ==&gt; specie_1[c] + specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: (2) specie_2 ==&gt; specie_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_2 + (2) specie_3 ==&gt; specie_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reaction_name_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[c]: specie_4 ==&gt; (2) specie_5 + specie_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Equation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">k_cat * specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c] / k_m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">backward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coefficient</t>
   </si>
   <si>
@@ -438,12 +459,6 @@
   </si>
   <si>
     <t xml:space="preserve">biomass_comp_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism biomass reaction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No comment</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
@@ -631,7 +646,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -650,10 +665,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -689,11 +700,23 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -908,19 +931,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -931,16 +954,16 @@
     </row>
     <row r="2" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>0</v>
@@ -952,20 +975,20 @@
         <v>1</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="10"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
@@ -977,20 +1000,20 @@
         <v>2</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -1000,16 +1023,16 @@
     </row>
     <row r="5" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>91</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>0</v>
@@ -1049,19 +1072,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -1072,80 +1095,80 @@
     </row>
     <row r="2" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="0"/>
       <c r="E2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="5" t="n">
         <v>2000</v>
       </c>
       <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" s="5" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="5" t="n">
         <v>0.001</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D5" s="6" t="n">
+        <v>102</v>
+      </c>
+      <c r="D5" s="5" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="5" t="n">
         <v>0.001</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="6" t="n">
+        <v>65</v>
+      </c>
+      <c r="D6" s="5" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="5" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -1165,94 +1188,51 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="12" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="11" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="15" t="n">
-        <v>-3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="15" t="n">
-        <v>-4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1271,47 +1251,101 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="12" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="13" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="13" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="12" t="s">
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="16" t="n">
+        <v>-3</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="16" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>114</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1356,10 +1390,10 @@
         <v>116</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>13</v>
@@ -1426,7 +1460,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1480,7 +1514,7 @@
         <v>124</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>125</v>
@@ -1561,16 +1595,16 @@
         <v>136</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>137</v>
@@ -1659,15 +1693,19 @@
   </sheetPr>
   <dimension ref="1:3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1022" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1021" min="1" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1684,44 +1722,39 @@
         <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AMI1" s="1"/>
+      <c r="AMH1" s="1"/>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1760,7 +1793,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -1772,30 +1805,30 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>4.58E-017</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="6" t="n">
-        <v>4.58E-017</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>1E-012</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="6" t="n">
-        <v>1E-012</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1836,19 +1869,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -1860,13 +1893,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>1</v>
@@ -1874,20 +1907,20 @@
       <c r="F2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="7"/>
+      <c r="G2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>2</v>
@@ -1895,20 +1928,20 @@
       <c r="F3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="7"/>
+      <c r="G3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>3</v>
@@ -1916,20 +1949,20 @@
       <c r="F4" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="7"/>
+      <c r="G4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>4</v>
@@ -1937,20 +1970,20 @@
       <c r="F5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="7"/>
+      <c r="G5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>5</v>
@@ -1958,20 +1991,20 @@
       <c r="F6" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="7"/>
+      <c r="G6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>6</v>
@@ -1979,8 +2012,8 @@
       <c r="F7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>46</v>
+      <c r="G7" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2013,116 +2046,116 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="C1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>43</v>
+        <v>62</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>47</v>
+        <v>63</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>43</v>
+        <v>64</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>47</v>
+        <v>65</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>50</v>
+        <v>66</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>53</v>
+        <v>67</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>56</v>
+        <v>68</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>59</v>
+        <v>69</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2143,7 +2176,7 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -2155,13 +2188,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -2172,68 +2205,68 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="7" t="n">
+        <v>62</v>
+      </c>
+      <c r="B2" s="6" t="n">
         <v>0.000148</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>75</v>
+      <c r="C2" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="7" t="n">
+        <v>63</v>
+      </c>
+      <c r="B3" s="6" t="n">
         <v>0.0002</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>75</v>
+      <c r="C3" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="7" t="n">
+        <v>65</v>
+      </c>
+      <c r="B4" s="6" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>75</v>
+      <c r="C4" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="7" t="n">
+        <v>67</v>
+      </c>
+      <c r="B5" s="6" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>75</v>
+      <c r="C5" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="7" t="n">
+        <v>68</v>
+      </c>
+      <c r="B6" s="6" t="n">
         <v>0.001</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>75</v>
+      <c r="C6" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="7" t="n">
+        <v>69</v>
+      </c>
+      <c r="B7" s="6" t="n">
         <v>0.002</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>75</v>
+      <c r="C7" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2272,7 +2305,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -2314,7 +2347,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
refactoring dFBA objective; adding references to observables, functions, and stop conditions; adding id to RateLaw
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_check_model_model.xlsx
+++ b/tests/fixtures/test_check_model_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,20 +17,21 @@
     <sheet name="Concentrations" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Observables" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="Functions" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Reactions" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="Rate laws" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="Biomass reactions" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Biomass components" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Parameters" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="Stop conditions" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="References" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="Database references" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="dFBA objectives" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Reactions" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="Rate laws" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="Biomass reactions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="Biomass components" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Parameters" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="Stop conditions" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="References" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="Database references" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="true" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
@@ -47,6 +48,11 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
@@ -61,48 +67,68 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="9" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="15" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -114,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="143">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -179,9 +205,6 @@
     <t xml:space="preserve">Algorithm</t>
   </si>
   <si>
-    <t xml:space="preserve">Objective function</t>
-  </si>
-  <si>
     <t xml:space="preserve">dfba_submodel</t>
   </si>
   <si>
@@ -191,159 +214,162 @@
     <t xml:space="preserve">dfba</t>
   </si>
   <si>
+    <t xml:space="preserve">ssa_submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNA degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracellular space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typical density of Mycoplasma pneumoniae cells in culture is 1e-9 cells/mL [Ref-0002].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empirical formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molecular weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pseudo_species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N2O2Na3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H3SO4C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_name_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_1[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_3[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_4[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_5[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specie_6[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submodel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-obj-dfba_submodel</t>
+  </si>
+  <si>
     <t xml:space="preserve">2*Metabolism_biomass</t>
   </si>
   <si>
-    <t xml:space="preserve">ssa_submodel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RNA degradation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ssa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extracellular space</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typical density of Mycoplasma pneumoniae cells in culture is 1e-9 cells/mL [Ref-0002].</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Empirical formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molecular weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pseudo_species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N2O2Na3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H3SO4C9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_name_6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U238</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2[e]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_1[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_2[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_3[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_4[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_5[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specie_6[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submodel</t>
-  </si>
-  <si>
     <t xml:space="preserve">Participants</t>
   </si>
   <si>
@@ -407,22 +433,37 @@
     <t xml:space="preserve">K m</t>
   </si>
   <si>
+    <t xml:space="preserve">reaction_1-forward</t>
+  </si>
+  <si>
     <t xml:space="preserve">forward</t>
   </si>
   <si>
     <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
   </si>
   <si>
+    <t xml:space="preserve">reaction_2-forward</t>
+  </si>
+  <si>
     <t xml:space="preserve">k_cat * specie_2[c]</t>
   </si>
   <si>
+    <t xml:space="preserve">reaction_3-forward</t>
+  </si>
+  <si>
     <t xml:space="preserve">specie_4[c] / k_m</t>
   </si>
   <si>
+    <t xml:space="preserve">reaction_3-backward</t>
+  </si>
+  <si>
     <t xml:space="preserve">backward</t>
   </si>
   <si>
     <t xml:space="preserve">specie_5[c] + specie_6[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction_4-forward</t>
   </si>
   <si>
     <t xml:space="preserve">Metabolism_biomass</t>
@@ -683,6 +724,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -713,10 +758,6 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -909,6 +950,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="9" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="9" width="9.10526315789474"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -931,7 +1037,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>76</v>
@@ -960,7 +1066,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>82</v>
@@ -975,7 +1081,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="9"/>
+      <c r="I2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -985,7 +1091,7 @@
         <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>85</v>
@@ -1000,7 +1106,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="9"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -1010,7 +1116,7 @@
         <v>87</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>88</v>
@@ -1029,9 +1135,9 @@
         <v>90</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>91</v>
       </c>
       <c r="E5" s="1" t="n">
@@ -1053,122 +1159,144 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="5" t="n">
         <v>2000</v>
       </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="5" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="G4" s="5" t="n">
         <v>0.001</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="5" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="G5" s="5" t="n">
         <v>0.001</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="5" t="n">
         <v>0.0003</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="G6" s="5" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -1183,14 +1311,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
@@ -1200,39 +1328,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="11" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="12" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>105</v>
+      <c r="A2" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +1374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1263,89 +1391,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="13" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="16.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="13" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="14" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="14" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="15" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" s="16" t="n">
+      <c r="D2" s="17" t="n">
         <v>-3</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="17" t="n">
+        <v>-4</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D3" s="16" t="n">
-        <v>-4</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1359,7 +1487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1384,16 +1512,16 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>13</v>
@@ -1404,10 +1532,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -1416,10 +1544,10 @@
         <v>0.3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1435,15 +1563,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M39" activeCellId="0" sqref="M39"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1452,7 +1580,7 @@
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1460,10 +1588,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1477,7 +1608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1502,46 +1633,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>13</v>
@@ -1561,7 +1692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1580,34 +1711,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>92</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1703,9 +1834,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1021" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1020" min="1" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1021" min="1021" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1719,42 +1850,37 @@
         <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AMH1" s="1"/>
+      <c r="AMG1" s="1"/>
+      <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1793,7 +1919,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -1805,30 +1931,30 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>4.58E-017</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>1E-012</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1869,19 +1995,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -1893,13 +2019,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>1</v>
@@ -1908,19 +2034,19 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>2</v>
@@ -1929,19 +2055,19 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>3</v>
@@ -1950,19 +2076,19 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>4</v>
@@ -1971,19 +2097,19 @@
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>5</v>
@@ -1992,19 +2118,19 @@
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>6</v>
@@ -2013,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2046,7 +2172,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -2058,10 +2184,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>13</v>
@@ -2072,90 +2198,90 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2177,7 +2303,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2188,13 +2314,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
@@ -2205,68 +2331,68 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>0.000148</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>0.0002</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>0.0005</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>0.0005</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>0.001</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B7" s="6" t="n">
         <v>0.002</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2285,10 +2411,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2305,10 +2431,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2327,10 +2456,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2339,7 +2468,7 @@
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2347,10 +2476,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring expressions adding id and name columns to RateLaw and Concentration deleting model, submodel columns of Parameter moving dFBA objectives to separate worksheet correcting plurality of relationships adding reference columns to observables, functions, stop conditions
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_check_model_model.xlsx
+++ b/tests/fixtures/test_check_model_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
@@ -53,6 +53,8 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
@@ -72,6 +74,8 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -91,25 +95,29 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$F$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -129,6 +137,8 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -140,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="148">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -355,9 +365,27 @@
     <t xml:space="preserve">Units</t>
   </si>
   <si>
+    <t xml:space="preserve">conc-specie_1[e]</t>
+  </si>
+  <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
+    <t xml:space="preserve">conc-specie_2[e]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_2[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_4[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_5[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conc-specie_6[c]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Expression</t>
   </si>
   <si>
@@ -427,12 +455,6 @@
     <t xml:space="preserve">Equation</t>
   </si>
   <si>
-    <t xml:space="preserve">K cat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K m</t>
-  </si>
-  <si>
     <t xml:space="preserve">reaction_1-forward</t>
   </si>
   <si>
@@ -445,13 +467,13 @@
     <t xml:space="preserve">reaction_2-forward</t>
   </si>
   <si>
-    <t xml:space="preserve">k_cat * specie_2[c]</t>
+    <t xml:space="preserve">k_cat_2 * specie_2[c]</t>
   </si>
   <si>
     <t xml:space="preserve">reaction_3-forward</t>
   </si>
   <si>
-    <t xml:space="preserve">specie_4[c] / k_m</t>
+    <t xml:space="preserve">specie_4[c] / k_m_3</t>
   </si>
   <si>
     <t xml:space="preserve">reaction_3-backward</t>
@@ -502,67 +524,70 @@
     <t xml:space="preserve">biomass_comp_3</t>
   </si>
   <si>
+    <t xml:space="preserve">fractionDryWeight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of cell mass which is non water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dimensionless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Ref-0006]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_cat_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k_m_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publisher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">Model</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submodels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fractionDryWeight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fraction of cell mass which is non water</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dimensionless</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Ref-0006]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Publisher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Series</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chapter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
   </si>
   <si>
     <t xml:space="preserve">Taxon</t>
@@ -962,9 +987,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="9" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="39.9554655870445"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="40.5991902834008"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="9" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -976,10 +1001,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>13</v>
@@ -990,13 +1015,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1018,7 +1043,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1037,19 +1062,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -1060,16 +1085,16 @@
     </row>
     <row r="2" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>0</v>
@@ -1085,16 +1110,16 @@
     </row>
     <row r="3" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
@@ -1110,16 +1135,16 @@
     </row>
     <row r="4" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -1129,16 +1154,16 @@
     </row>
     <row r="5" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>0</v>
@@ -1164,140 +1189,113 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F2" s="0"/>
+        <v>103</v>
+      </c>
       <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="G3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0.0003</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>107</v>
+      </c>
+      <c r="G4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.0003</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0.0003</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0.001</v>
       </c>
     </row>
   </sheetData>
@@ -1340,7 +1338,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>13</v>
@@ -1351,16 +1349,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1390,7 @@
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="14" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="17.5668016194332"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="14" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="14" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="15" width="8.78542510121457"/>
@@ -1406,10 +1404,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>68</v>
@@ -1423,13 +1421,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D2" s="17" t="n">
         <v>-3</v>
@@ -1438,19 +1436,19 @@
         <v>62</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D3" s="17" t="n">
         <v>-4</v>
@@ -1461,13 +1459,13 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D4" s="17" t="n">
         <v>1</v>
@@ -1492,16 +1490,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1512,46 +1510,57 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="n">
+        <v>125</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>125</v>
+      <c r="D2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="0"/>
+      <c r="C3" s="5" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="0"/>
+      <c r="C4" s="5" t="n">
+        <v>0.001</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:D1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1588,7 +1597,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1633,46 +1642,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>38</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>13</v>
@@ -1711,22 +1720,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>59</v>
@@ -1735,10 +1744,10 @@
         <v>58</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2300,99 +2309,124 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="D2" s="6" t="n">
         <v>0.000148</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>71</v>
+      <c r="E2" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="D3" s="6" t="n">
         <v>0.0002</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>71</v>
+      <c r="E3" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="D4" s="6" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>71</v>
+      <c r="E4" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="D5" s="6" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>71</v>
+      <c r="E5" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="D6" s="6" t="n">
         <v>0.001</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>71</v>
+      <c r="E6" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="D7" s="6" t="n">
         <v>0.002</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>71</v>
+      <c r="E7" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2431,7 +2465,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -2476,7 +2510,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
adding CompartmentType and type attribute to Compartment
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_check_model_model.xlsx
+++ b/tests/fixtures/test_check_model_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,33 +28,34 @@
     <sheet name="Database references" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">submodels!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$D$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
@@ -76,6 +77,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -97,6 +99,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
@@ -118,6 +121,7 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -139,6 +143,7 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -150,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="149">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -233,6 +238,9 @@
     <t xml:space="preserve">ssa</t>
   </si>
   <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Initial volume</t>
   </si>
   <si>
@@ -242,6 +250,9 @@
     <t xml:space="preserve">Cell</t>
   </si>
   <si>
+    <t xml:space="preserve">physical_3d</t>
+  </si>
+  <si>
     <t xml:space="preserve">Average volume of Mycoplasma pneumoniae is 66 aL [Ref-0001]. This equates to 45.8 aL at the beginning of the cell cycle (66 aL * ln(2)).</t>
   </si>
   <si>
@@ -264,9 +275,6 @@
   </si>
   <si>
     <t xml:space="preserve">Charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
   </si>
   <si>
     <t xml:space="preserve">specie_1</t>
@@ -886,7 +894,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -982,14 +990,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="1" sqref="C3 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="9" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="40.5991902834008"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="40.919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="9" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1001,10 +1009,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>13</v>
@@ -1015,13 +1023,13 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1062,19 +1070,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -1085,16 +1093,16 @@
     </row>
     <row r="2" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>0</v>
@@ -1110,16 +1118,16 @@
     </row>
     <row r="3" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
@@ -1135,16 +1143,16 @@
     </row>
     <row r="4" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -1154,16 +1162,16 @@
     </row>
     <row r="5" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>0</v>
@@ -1192,7 +1200,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="C3 G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1210,13 +1218,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -1227,75 +1235,75 @@
     </row>
     <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1321,7 +1329,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D7" activeCellId="1" sqref="C3 D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1338,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>13</v>
@@ -1349,16 +1357,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1384,13 +1392,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="C7" activeCellId="1" sqref="C3 C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="14" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="14" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="14" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="15" width="8.78542510121457"/>
@@ -1404,13 +1412,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>13</v>
@@ -1421,57 +1429,57 @@
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D2" s="17" t="n">
         <v>-3</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" s="17" t="n">
         <v>-4</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D4" s="17" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1492,8 +1500,8 @@
   </sheetPr>
   <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="C3 F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1510,10 +1518,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>13</v>
@@ -1526,24 +1534,24 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>0.3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B3" s="0"/>
       <c r="C3" s="5" t="n">
@@ -1552,7 +1560,7 @@
     </row>
     <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="5" t="n">
@@ -1580,7 +1588,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="C3 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1597,7 +1605,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1625,7 +1633,7 @@
   <dimension ref="1:1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="1" sqref="C3 F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1642,46 +1650,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>13</v>
@@ -1709,7 +1717,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="C3 E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1720,34 +1728,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1769,7 +1777,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+      <selection pane="topLeft" activeCell="C36" activeCellId="1" sqref="C3 C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1838,7 +1846,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="1" sqref="C3 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1908,16 +1916,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="3" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1931,43 +1938,51 @@
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AMJ1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="5" t="n">
         <v>4.58E-017</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>30</v>
+      <c r="E2" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="5" t="n">
+      <c r="D3" s="5" t="n">
         <v>1E-012</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>33</v>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D3"/>
+  <autoFilter ref="A1:E3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1987,7 +2002,7 @@
   <dimension ref="1:7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="1" sqref="C3 E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2004,19 +2019,19 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>13</v>
@@ -2028,13 +2043,13 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>1</v>
@@ -2043,19 +2058,19 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>2</v>
@@ -2064,19 +2079,19 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>3</v>
@@ -2085,19 +2100,19 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>4</v>
@@ -2106,19 +2121,19 @@
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>5</v>
@@ -2127,19 +2142,19 @@
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>6</v>
@@ -2148,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2176,7 +2191,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="bottomRight" activeCell="B13" activeCellId="1" sqref="C3 B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2193,10 +2208,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>13</v>
@@ -2207,90 +2222,90 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2312,7 +2327,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C3 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2330,13 +2345,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -2347,86 +2362,86 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2" s="6" t="n">
         <v>0.000148</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>0.0002</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>0.0005</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>0.0005</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>0.001</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>0.002</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2448,7 +2463,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C3 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2465,7 +2480,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -2493,7 +2508,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C3 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2510,7 +2525,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
- add author, author organization, author email, created, updated meta data to Model - add type to Parameter - add type, units to RateLaw
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_check_model_model.xlsx
+++ b/tests/fixtures/test_check_model_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
@@ -56,6 +56,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$E$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
@@ -78,6 +79,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
@@ -100,28 +102,30 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$D$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$E$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
@@ -144,6 +148,7 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -155,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="157">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -196,9 +201,24 @@
     <t xml:space="preserve">wc_lang version</t>
   </si>
   <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author email</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
+    <t xml:space="preserve">Created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated</t>
+  </si>
+  <si>
     <t xml:space="preserve">ASP_test</t>
   </si>
   <si>
@@ -469,9 +489,15 @@
     <t xml:space="preserve">forward</t>
   </si>
   <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
     <t xml:space="preserve">max( specie_1[e], specie_2[e] )</t>
   </si>
   <si>
+    <t xml:space="preserve">s^-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">reaction_2-forward</t>
   </si>
   <si>
@@ -547,13 +573,16 @@
     <t xml:space="preserve">k_cat_2</t>
   </si>
   <si>
+    <t xml:space="preserve">k_cat</t>
+  </si>
+  <si>
     <t xml:space="preserve">k_m_3</t>
   </si>
   <si>
+    <t xml:space="preserve">K_m</t>
+  </si>
+  <si>
     <t xml:space="preserve">Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Author</t>
   </si>
   <si>
     <t xml:space="preserve">Editor</t>
@@ -891,10 +920,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C3 A1"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -959,9 +988,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -990,14 +1044,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="1" sqref="C3 A3"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="9" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="41.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="9" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1009,27 +1063,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1070,39 +1124,39 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="112" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>0</v>
@@ -1118,16 +1172,16 @@
     </row>
     <row r="3" customFormat="false" ht="56" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
@@ -1143,16 +1197,16 @@
     </row>
     <row r="4" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>1</v>
@@ -1162,16 +1216,16 @@
     </row>
     <row r="5" customFormat="false" ht="84" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>0</v>
@@ -1197,20 +1251,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="1" sqref="C3 G3"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1218,92 +1270,125 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="E6" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1329,7 +1414,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" activeCellId="1" sqref="C3 D7"/>
+      <selection pane="bottomRight" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1346,27 +1431,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1392,13 +1477,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C7" activeCellId="1" sqref="C3 C7"/>
+      <selection pane="bottomRight" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="14" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="14" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="14" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="15" width="8.78542510121457"/>
@@ -1412,74 +1497,74 @@
         <v>2</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D2" s="17" t="n">
         <v>-3</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="G2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D3" s="17" t="n">
         <v>-4</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D4" s="17" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1500,17 +1585,21 @@
   </sheetPr>
   <dimension ref="1:4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="1" sqref="C3 F8"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1518,57 +1607,68 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AMJ1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="3" t="n">
+        <v>133</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="E2" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>134</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="0"/>
-      <c r="C3" s="5" t="n">
+        <v>136</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="5" t="n">
         <v>2000</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" s="0"/>
-      <c r="C4" s="5" t="n">
+        <v>138</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="5" t="n">
         <v>0.001</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:E1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1588,7 +1688,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="C3 E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1605,13 +1705,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +1733,7 @@
   <dimension ref="1:1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="1" sqref="C3 F32"/>
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1650,49 +1750,49 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AMJ1" s="1"/>
     </row>
@@ -1717,7 +1817,7 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="C3 E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1728,34 +1828,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1777,7 +1877,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C36" activeCellId="1" sqref="C3 C36"/>
+      <selection pane="topLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1791,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1799,28 +1899,28 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1846,7 +1946,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="1" sqref="C3 A2"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1864,13 +1964,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="AMG1" s="1"/>
       <c r="AMH1" s="0"/>
@@ -1879,25 +1979,25 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1918,7 +2018,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1935,50 +2035,50 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D2" s="5" t="n">
         <v>4.58E-017</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D3" s="5" t="n">
         <v>1E-012</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2002,7 +2102,7 @@
   <dimension ref="1:7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="1" sqref="C3 E39"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2019,37 +2119,37 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="AMJ1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>1</v>
@@ -2058,19 +2158,19 @@
         <v>0</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>2</v>
@@ -2079,19 +2179,19 @@
         <v>0</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>3</v>
@@ -2100,19 +2200,19 @@
         <v>0</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>4</v>
@@ -2121,19 +2221,19 @@
         <v>0</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>5</v>
@@ -2142,19 +2242,19 @@
         <v>0</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>6</v>
@@ -2163,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2191,7 +2291,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B13" activeCellId="1" sqref="C3 B13"/>
+      <selection pane="bottomRight" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2208,104 +2308,104 @@
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2327,7 +2427,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2345,103 +2445,103 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D2" s="6" t="n">
         <v>0.000148</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>0.0002</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>0.0005</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>0.0005</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>0.001</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>0.002</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2463,7 +2563,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C3 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2480,13 +2580,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2508,7 +2608,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="C3 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2525,13 +2625,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>